<commit_message>
Reading new data from Anjana in Ch9.
</commit_message>
<xml_diff>
--- a/chapters/ch09-Agriculture/datasets/Energy Flow in the US Food System.xlsx
+++ b/chapters/ch09-Agriculture/datasets/Energy Flow in the US Food System.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch09-Agriculture/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38504684-67C4-0541-ABB7-DA450647A0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B7DA38-8269-744B-9BC6-A27049ADEC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8380" yWindow="820" windowWidth="28920" windowHeight="24820" xr2:uid="{E5BEA42B-B012-4EC3-A8FA-62205E68D6FA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Energy Flow in the US Food System</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Consumed energy [quads]</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -504,6 +507,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
       <c r="B1" t="s">
         <v>14</v>
       </c>

</xml_diff>